<commit_message>
feature - sql aprovado
</commit_message>
<xml_diff>
--- a/arquivos-diagramas/Extrato_De_Horas_Implementação.xlsx
+++ b/arquivos-diagramas/Extrato_De_Horas_Implementação.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agostinho.junior\Documents\GitHub\Mercado\arquivos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\william.mauro\Documents\GitHub\Vin-Diesel\arquivos-diagramas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -223,9 +223,6 @@
     <t>Fabricar História de Produto</t>
   </si>
   <si>
-    <t>Fabricar História de Gerenciar Produtos (Inserir,Editar,Listar e Excluir)</t>
-  </si>
-  <si>
     <t>Fabricar História de Receita</t>
   </si>
   <si>
@@ -575,6 +572,9 @@
   </si>
   <si>
     <t>RNF-19</t>
+  </si>
+  <si>
+    <t>Fabricar História de Gerenciar Encomendas (Inserir,Editar,Listar e Excluir)</t>
   </si>
 </sst>
 </file>
@@ -1044,8 +1044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C44" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1077,7 +1077,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G1" s="16" t="s">
         <v>4</v>
@@ -1113,7 +1113,7 @@
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -1141,7 +1141,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>57</v>
@@ -1161,7 +1161,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>60</v>
@@ -1181,13 +1181,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>64</v>
+        <v>181</v>
       </c>
       <c r="D6" s="4">
         <v>2</v>
@@ -1201,13 +1201,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>75</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>76</v>
       </c>
       <c r="D7" s="4">
         <v>2</v>
@@ -1221,13 +1221,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>65</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>66</v>
       </c>
       <c r="D8" s="4">
         <v>2</v>
@@ -1241,13 +1241,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>68</v>
       </c>
       <c r="D9" s="4">
         <v>2</v>
@@ -1261,13 +1261,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>69</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>70</v>
       </c>
       <c r="D10" s="4">
         <v>2</v>
@@ -1281,13 +1281,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D11" s="4">
         <v>2</v>
@@ -1301,13 +1301,13 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>73</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>74</v>
       </c>
       <c r="D12" s="4">
         <v>2</v>
@@ -1321,13 +1321,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D13" s="4">
         <v>2</v>
@@ -1341,7 +1341,7 @@
     </row>
     <row r="14" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>11</v>
@@ -1368,7 +1368,7 @@
     </row>
     <row r="15" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>13</v>
@@ -1395,7 +1395,7 @@
     </row>
     <row r="16" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>15</v>
@@ -1422,7 +1422,7 @@
     </row>
     <row r="17" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>17</v>
@@ -1450,13 +1450,13 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
@@ -1470,13 +1470,13 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D19" s="4">
         <v>1</v>
@@ -1490,13 +1490,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D20" s="4">
         <v>2</v>
@@ -1510,13 +1510,13 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D21" s="4">
         <v>2</v>
@@ -1530,13 +1530,13 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D22" s="4">
         <v>2</v>
@@ -1550,13 +1550,13 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D23" s="4">
         <v>2</v>
@@ -1570,13 +1570,13 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D24" s="4">
         <v>2</v>
@@ -1590,13 +1590,13 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D25" s="4">
         <v>2</v>
@@ -1610,13 +1610,13 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D26" s="4">
         <v>2</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D27" s="4">
         <v>2</v>
@@ -1650,7 +1650,7 @@
     </row>
     <row r="28" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>20</v>
@@ -1677,7 +1677,7 @@
     </row>
     <row r="29" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>22</v>
@@ -1704,7 +1704,7 @@
     </row>
     <row r="30" spans="1:8" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>24</v>
@@ -1731,7 +1731,7 @@
     </row>
     <row r="31" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>26</v>
@@ -1759,13 +1759,13 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D32" s="4">
         <v>2</v>
@@ -1779,13 +1779,13 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D33" s="4">
         <v>3</v>
@@ -1799,13 +1799,13 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D34" s="4">
         <v>3</v>
@@ -1819,13 +1819,13 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C35" s="6" t="s">
         <v>123</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>124</v>
       </c>
       <c r="D35" s="4">
         <v>3</v>
@@ -1839,13 +1839,13 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B36" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>130</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>131</v>
       </c>
       <c r="D36" s="4">
         <v>3</v>
@@ -1859,13 +1859,13 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="C37" s="6" t="s">
         <v>133</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>134</v>
       </c>
       <c r="D37" s="4">
         <v>1</v>
@@ -1879,7 +1879,7 @@
     </row>
     <row r="38" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>29</v>
@@ -1906,7 +1906,7 @@
     </row>
     <row r="39" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>32</v>
@@ -1933,7 +1933,7 @@
     </row>
     <row r="40" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>35</v>
@@ -1961,13 +1961,13 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D41" s="4">
         <v>1</v>
@@ -1981,13 +1981,13 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D42" s="4">
         <v>1</v>
@@ -2001,13 +2001,13 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D43" s="4">
         <v>1</v>
@@ -2021,13 +2021,13 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D44" s="4">
         <v>1</v>
@@ -2041,13 +2041,13 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D45" s="4">
         <v>1</v>
@@ -2061,13 +2061,13 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D46" s="4">
         <v>1</v>
@@ -2081,13 +2081,13 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D47" s="4">
         <v>1</v>
@@ -2101,13 +2101,13 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D48" s="4">
         <v>1</v>
@@ -2121,13 +2121,13 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C49" s="6" t="s">
         <v>153</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>154</v>
       </c>
       <c r="D49" s="4">
         <v>1</v>
@@ -2141,13 +2141,13 @@
     </row>
     <row r="50" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D50" s="4">
         <v>1</v>
@@ -2161,7 +2161,7 @@
     </row>
     <row r="51" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>37</v>
@@ -2182,13 +2182,13 @@
         <v>8</v>
       </c>
       <c r="H51" s="14">
-        <f t="shared" ref="H50:H57" si="0">D51*E51</f>
+        <f t="shared" ref="H51:H57" si="0">D51*E51</f>
         <v>240</v>
       </c>
     </row>
     <row r="52" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>39</v>
@@ -2215,7 +2215,7 @@
     </row>
     <row r="53" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>41</v>
@@ -2242,7 +2242,7 @@
     </row>
     <row r="54" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>43</v>
@@ -2269,7 +2269,7 @@
     </row>
     <row r="55" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>45</v>
@@ -2296,7 +2296,7 @@
     </row>
     <row r="56" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>48</v>
@@ -2323,13 +2323,13 @@
     </row>
     <row r="57" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B57" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C57" s="5" t="s">
         <v>156</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>157</v>
       </c>
       <c r="D57" s="2">
         <v>8</v>
@@ -2348,7 +2348,7 @@
     </row>
     <row r="58" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>50</v>
@@ -2403,7 +2403,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D61" s="18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G61" s="3"/>
       <c r="H61" s="8"/>

</xml_diff>